<commit_message>
patient appointment with missing field of date andmessage is added
</commit_message>
<xml_diff>
--- a/SmartHospitals_Cucumber/src/test/resources/Book2.xlsx
+++ b/SmartHospitals_Cucumber/src/test/resources/Book2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SmartHospital\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhanusheswaran M\git\Smart_Hospital_Cucumber_Project\SmartHospitals_Cucumber\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDA0EAD9-4F1B-43D9-B2AD-0CF30AE581E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE58E1D-E8B0-46CC-BC46-501409467C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB9F6582-CA60-48AE-A3D3-0072BC22671A}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +77,13 @@
       <color theme="1"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -99,10 +106,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="18" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,20 +431,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63B02C7B-F73A-4DD6-92B4-9BBB93ED6131}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="7" max="7" width="17.5546875" customWidth="1"/>
-    <col min="8" max="8" width="14.21875" customWidth="1"/>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="72.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.6640625" customWidth="1"/>
-    <col min="10" max="10" width="22.77734375" customWidth="1"/>
-    <col min="11" max="11" width="13.21875" customWidth="1"/>
-    <col min="12" max="12" width="14.88671875" customWidth="1"/>
+    <col min="10" max="10" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
@@ -567,6 +587,69 @@
         <v>7</v>
       </c>
     </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="4"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
patient appointment with missing field is corrected in data empty field
</commit_message>
<xml_diff>
--- a/SmartHospitals_Cucumber/src/test/resources/Book2.xlsx
+++ b/SmartHospitals_Cucumber/src/test/resources/Book2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhanusheswaran M\git\Smart_Hospital_Cucumber_Project\SmartHospitals_Cucumber\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDE58E1D-E8B0-46CC-BC46-501409467C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5BFC9BB-6681-460C-AEDB-5A5CDECA3A2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CB9F6582-CA60-48AE-A3D3-0072BC22671A}"/>
   </bookViews>
@@ -434,7 +434,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>